<commit_message>
Final version hypatia teaching
</commit_message>
<xml_diff>
--- a/hypatia/examples/Planning_teaching/parameters/parameters_global.xlsx
+++ b/hypatia/examples/Planning_teaching/parameters/parameters_global.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://polimi365-my.sharepoint.com/personal/10530003_polimi_it/Documents/Research/MODELS/Hypatia_teaching_version/hypatia/examples/Planning_teaching/parameters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="11_518BC36504AB7D5137B74E85F1507E2B41951101" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BC65C491-AE47-47A2-A7D2-1AD929B28C34}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="11_518BC36504AB7D5137B74E85F1507E2B41951101" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CC8EA0DA-E309-4196-BC2B-60E962D4C9CB}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="12" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Discount_rate" sheetId="1" r:id="rId1"/>
@@ -26,13 +26,14 @@
     <sheet name="Renewable_tech_selection" sheetId="11" r:id="rId11"/>
     <sheet name="Global_Min_RES_production" sheetId="12" r:id="rId12"/>
     <sheet name="Global_Min_RES_elec_penetration" sheetId="13" r:id="rId13"/>
+    <sheet name="Max_land_usage_global" sheetId="14" r:id="rId14"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="36">
   <si>
     <t>Years</t>
   </si>
@@ -146,7 +147,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -159,6 +160,11 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -196,12 +202,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1426,6 +1435,475 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27FD3D0B-A051-4F90-85E1-F39B77C92FF9}">
+  <dimension ref="A1:L12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>1E+30</v>
+      </c>
+      <c r="C2">
+        <v>1E+30</v>
+      </c>
+      <c r="D2">
+        <v>1E+30</v>
+      </c>
+      <c r="E2">
+        <v>1E+30</v>
+      </c>
+      <c r="F2">
+        <v>1E+30</v>
+      </c>
+      <c r="G2">
+        <v>1E+30</v>
+      </c>
+      <c r="H2">
+        <v>1E+30</v>
+      </c>
+      <c r="I2">
+        <v>1E+30</v>
+      </c>
+      <c r="J2">
+        <v>1E+30</v>
+      </c>
+      <c r="K2">
+        <v>1E+30</v>
+      </c>
+      <c r="L2">
+        <v>1E+30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>1E+30</v>
+      </c>
+      <c r="C3">
+        <v>1E+30</v>
+      </c>
+      <c r="D3">
+        <v>1E+30</v>
+      </c>
+      <c r="E3">
+        <v>1E+30</v>
+      </c>
+      <c r="F3">
+        <v>1E+30</v>
+      </c>
+      <c r="G3">
+        <v>1E+30</v>
+      </c>
+      <c r="H3">
+        <v>1E+30</v>
+      </c>
+      <c r="I3">
+        <v>1E+30</v>
+      </c>
+      <c r="J3">
+        <v>1E+30</v>
+      </c>
+      <c r="K3">
+        <v>1E+30</v>
+      </c>
+      <c r="L3">
+        <v>1E+30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>1E+30</v>
+      </c>
+      <c r="C4">
+        <v>1E+30</v>
+      </c>
+      <c r="D4">
+        <v>1E+30</v>
+      </c>
+      <c r="E4">
+        <v>1E+30</v>
+      </c>
+      <c r="F4">
+        <v>1E+30</v>
+      </c>
+      <c r="G4">
+        <v>1E+30</v>
+      </c>
+      <c r="H4">
+        <v>1E+30</v>
+      </c>
+      <c r="I4">
+        <v>1E+30</v>
+      </c>
+      <c r="J4">
+        <v>1E+30</v>
+      </c>
+      <c r="K4">
+        <v>1E+30</v>
+      </c>
+      <c r="L4">
+        <v>1E+30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>1E+30</v>
+      </c>
+      <c r="C5">
+        <v>1E+30</v>
+      </c>
+      <c r="D5">
+        <v>1E+30</v>
+      </c>
+      <c r="E5">
+        <v>1E+30</v>
+      </c>
+      <c r="F5">
+        <v>1E+30</v>
+      </c>
+      <c r="G5">
+        <v>1E+30</v>
+      </c>
+      <c r="H5">
+        <v>1E+30</v>
+      </c>
+      <c r="I5">
+        <v>1E+30</v>
+      </c>
+      <c r="J5">
+        <v>1E+30</v>
+      </c>
+      <c r="K5">
+        <v>1E+30</v>
+      </c>
+      <c r="L5">
+        <v>1E+30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>1E+30</v>
+      </c>
+      <c r="C6">
+        <v>1E+30</v>
+      </c>
+      <c r="D6">
+        <v>1E+30</v>
+      </c>
+      <c r="E6">
+        <v>1E+30</v>
+      </c>
+      <c r="F6">
+        <v>1E+30</v>
+      </c>
+      <c r="G6">
+        <v>1E+30</v>
+      </c>
+      <c r="H6">
+        <v>1E+30</v>
+      </c>
+      <c r="I6">
+        <v>1E+30</v>
+      </c>
+      <c r="J6">
+        <v>1E+30</v>
+      </c>
+      <c r="K6">
+        <v>1E+30</v>
+      </c>
+      <c r="L6">
+        <v>1E+30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>1E+30</v>
+      </c>
+      <c r="C7">
+        <v>1E+30</v>
+      </c>
+      <c r="D7">
+        <v>1E+30</v>
+      </c>
+      <c r="E7">
+        <v>1E+30</v>
+      </c>
+      <c r="F7">
+        <v>1E+30</v>
+      </c>
+      <c r="G7">
+        <v>1E+30</v>
+      </c>
+      <c r="H7">
+        <v>1E+30</v>
+      </c>
+      <c r="I7">
+        <v>1E+30</v>
+      </c>
+      <c r="J7">
+        <v>1E+30</v>
+      </c>
+      <c r="K7">
+        <v>1E+30</v>
+      </c>
+      <c r="L7">
+        <v>1E+30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>1E+30</v>
+      </c>
+      <c r="C8">
+        <v>1E+30</v>
+      </c>
+      <c r="D8">
+        <v>1E+30</v>
+      </c>
+      <c r="E8">
+        <v>1E+30</v>
+      </c>
+      <c r="F8">
+        <v>1E+30</v>
+      </c>
+      <c r="G8">
+        <v>1E+30</v>
+      </c>
+      <c r="H8">
+        <v>1E+30</v>
+      </c>
+      <c r="I8">
+        <v>1E+30</v>
+      </c>
+      <c r="J8">
+        <v>1E+30</v>
+      </c>
+      <c r="K8">
+        <v>1E+30</v>
+      </c>
+      <c r="L8">
+        <v>1E+30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>1E+30</v>
+      </c>
+      <c r="C9">
+        <v>1E+30</v>
+      </c>
+      <c r="D9">
+        <v>1E+30</v>
+      </c>
+      <c r="E9">
+        <v>1E+30</v>
+      </c>
+      <c r="F9">
+        <v>1E+30</v>
+      </c>
+      <c r="G9">
+        <v>1E+30</v>
+      </c>
+      <c r="H9">
+        <v>1E+30</v>
+      </c>
+      <c r="I9">
+        <v>1E+30</v>
+      </c>
+      <c r="J9">
+        <v>1E+30</v>
+      </c>
+      <c r="K9">
+        <v>1E+30</v>
+      </c>
+      <c r="L9">
+        <v>1E+30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <v>1E+30</v>
+      </c>
+      <c r="C10">
+        <v>1E+30</v>
+      </c>
+      <c r="D10">
+        <v>1E+30</v>
+      </c>
+      <c r="E10">
+        <v>1E+30</v>
+      </c>
+      <c r="F10">
+        <v>1E+30</v>
+      </c>
+      <c r="G10">
+        <v>1E+30</v>
+      </c>
+      <c r="H10">
+        <v>1E+30</v>
+      </c>
+      <c r="I10">
+        <v>1E+30</v>
+      </c>
+      <c r="J10">
+        <v>1E+30</v>
+      </c>
+      <c r="K10">
+        <v>1E+30</v>
+      </c>
+      <c r="L10">
+        <v>1E+30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11">
+        <v>1E+30</v>
+      </c>
+      <c r="C11">
+        <v>1E+30</v>
+      </c>
+      <c r="D11">
+        <v>1E+30</v>
+      </c>
+      <c r="E11">
+        <v>1E+30</v>
+      </c>
+      <c r="F11">
+        <v>1E+30</v>
+      </c>
+      <c r="G11">
+        <v>1E+30</v>
+      </c>
+      <c r="H11">
+        <v>1E+30</v>
+      </c>
+      <c r="I11">
+        <v>1E+30</v>
+      </c>
+      <c r="J11">
+        <v>1E+30</v>
+      </c>
+      <c r="K11">
+        <v>1E+30</v>
+      </c>
+      <c r="L11">
+        <v>1E+30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A12" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12">
+        <v>1E+30</v>
+      </c>
+      <c r="C12">
+        <v>1E+30</v>
+      </c>
+      <c r="D12">
+        <v>1E+30</v>
+      </c>
+      <c r="E12">
+        <v>1E+30</v>
+      </c>
+      <c r="F12">
+        <v>1E+30</v>
+      </c>
+      <c r="G12">
+        <v>1E+30</v>
+      </c>
+      <c r="H12">
+        <v>1E+30</v>
+      </c>
+      <c r="I12">
+        <v>1E+30</v>
+      </c>
+      <c r="J12">
+        <v>1E+30</v>
+      </c>
+      <c r="K12">
+        <v>1E+30</v>
+      </c>
+      <c r="L12">
+        <v>1E+30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B12"/>
@@ -2948,7 +3426,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2:L12"/>
     </sheetView>
   </sheetViews>

</xml_diff>